<commit_message>
Updates Distritos_Concelhos / Partidos
</commit_message>
<xml_diff>
--- a/Docs/Distritos_Concelhos.xlsx
+++ b/Docs/Distritos_Concelhos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eduardomaio/Desktop/Votometro-A-Volta-a-Portugal-em-Eleicoes/Docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Rodrigo\Desktop\Python\Votometro-A-Volta-a-Portugal-em-Eleicoes\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFEFB7D5-DF5C-A54F-961F-94DD3A7AD8DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA2ACE8-6B20-483D-B8CB-6D9A030FEDBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="34200" windowHeight="19920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -20,17 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -722,9 +711,6 @@
     <t>MIRA</t>
   </si>
   <si>
-    <t>MIRANDA DO CORVO</t>
-  </si>
-  <si>
     <t>MONTEMOR-O-VELHO</t>
   </si>
   <si>
@@ -984,6 +970,9 @@
   </si>
   <si>
     <t>FORA EUROPA</t>
+  </si>
+  <si>
+    <t>MCORVO</t>
   </si>
 </sst>
 </file>
@@ -1389,18 +1378,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C312"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A285" zoomScale="160" workbookViewId="0">
-      <selection activeCell="G309" sqref="G309"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="160" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1411,7 +1400,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>149</v>
       </c>
@@ -1422,7 +1411,7 @@
         <v>41936</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>149</v>
       </c>
@@ -1433,7 +1422,7 @@
         <v>22449</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>149</v>
       </c>
@@ -1444,7 +1433,7 @@
         <v>25583</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>149</v>
       </c>
@@ -1455,7 +1444,7 @@
         <v>19670</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>149</v>
       </c>
@@ -1466,7 +1455,7 @@
         <v>70221</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>149</v>
       </c>
@@ -1477,7 +1466,7 @@
         <v>14016</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>149</v>
       </c>
@@ -1488,7 +1477,7 @@
         <v>29326</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>149</v>
       </c>
@@ -1499,7 +1488,7 @@
         <v>24018</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>149</v>
       </c>
@@ -1510,7 +1499,7 @@
         <v>36248</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>149</v>
       </c>
@@ -1521,7 +1510,7 @@
         <v>17706</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>149</v>
       </c>
@@ -1532,7 +1521,7 @@
         <v>9918</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>149</v>
       </c>
@@ -1543,7 +1532,7 @@
         <v>60480</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>149</v>
       </c>
@@ -1554,7 +1543,7 @@
         <v>20898</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>149</v>
       </c>
@@ -1565,7 +1554,7 @@
         <v>50902</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>149</v>
       </c>
@@ -1576,7 +1565,7 @@
         <v>126650</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>149</v>
       </c>
@@ -1587,7 +1576,7 @@
         <v>19533</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>149</v>
       </c>
@@ -1598,7 +1587,7 @@
         <v>10307</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>149</v>
       </c>
@@ -1609,7 +1598,7 @@
         <v>22338</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>149</v>
       </c>
@@ -1620,7 +1609,7 @@
         <v>19887</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>169</v>
       </c>
@@ -1631,7 +1620,7 @@
         <v>7761</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>169</v>
       </c>
@@ -1642,7 +1631,7 @@
         <v>5982</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>169</v>
       </c>
@@ -1653,7 +1642,7 @@
         <v>1850</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>169</v>
       </c>
@@ -1664,7 +1653,7 @@
         <v>1262</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>169</v>
       </c>
@@ -1675,7 +1664,7 @@
         <v>28392</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>169</v>
       </c>
@@ -1686,7 +1675,7 @@
         <v>6029</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>169</v>
       </c>
@@ -1697,7 +1686,7 @@
         <v>3646</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>169</v>
       </c>
@@ -1708,7 +1697,7 @@
         <v>6195</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>169</v>
       </c>
@@ -1719,7 +1708,7 @@
         <v>5598</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>169</v>
       </c>
@@ -1730,7 +1719,7 @@
         <v>11796</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>169</v>
       </c>
@@ -1741,7 +1730,7 @@
         <v>19563</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>169</v>
       </c>
@@ -1752,7 +1741,7 @@
         <v>4172</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>169</v>
       </c>
@@ -1763,7 +1752,7 @@
         <v>12279</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>169</v>
       </c>
@@ -1774,7 +1763,7 @@
         <v>4577</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>183</v>
       </c>
@@ -1785,7 +1774,7 @@
         <v>17657</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>183</v>
       </c>
@@ -1796,7 +1785,7 @@
         <v>106669</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>183</v>
       </c>
@@ -1807,7 +1796,7 @@
         <v>167507</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>183</v>
       </c>
@@ -1818,7 +1807,7 @@
         <v>16812</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>183</v>
       </c>
@@ -1829,7 +1818,7 @@
         <v>17312</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>183</v>
       </c>
@@ -1840,7 +1829,7 @@
         <v>33418</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>183</v>
       </c>
@@ -1851,7 +1840,7 @@
         <v>50031</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>183</v>
       </c>
@@ -1862,7 +1851,7 @@
         <v>143222</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>183</v>
       </c>
@@ -1873,7 +1862,7 @@
         <v>21875</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>183</v>
       </c>
@@ -1884,7 +1873,7 @@
         <v>6483</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>183</v>
       </c>
@@ -1895,7 +1884,7 @@
         <v>12166</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>183</v>
       </c>
@@ -1906,7 +1895,7 @@
         <v>120524</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>183</v>
       </c>
@@ -1917,7 +1906,7 @@
         <v>44715</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>183</v>
       </c>
@@ -1928,7 +1917,7 @@
         <v>21772</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>197</v>
       </c>
@@ -1939,7 +1928,7 @@
         <v>5101</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>197</v>
       </c>
@@ -1950,7 +1939,7 @@
         <v>35311</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>197</v>
       </c>
@@ -1961,7 +1950,7 @@
         <v>5860</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>197</v>
       </c>
@@ -1972,7 +1961,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>197</v>
       </c>
@@ -1983,7 +1972,7 @@
         <v>17168</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>197</v>
       </c>
@@ -1994,7 +1983,7 @@
         <v>6995</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>197</v>
       </c>
@@ -2005,7 +1994,7 @@
         <v>22495</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>197</v>
       </c>
@@ -2016,7 +2005,7 @@
         <v>9640</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>197</v>
       </c>
@@ -2027,7 +2016,7 @@
         <v>7573</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>197</v>
       </c>
@@ -2038,7 +2027,7 @@
         <v>6600</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>197</v>
       </c>
@@ -2049,7 +2038,7 @@
         <v>5178</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>197</v>
       </c>
@@ -2060,7 +2049,7 @@
         <v>9304</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>209</v>
       </c>
@@ -2071,7 +2060,7 @@
         <v>5844</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>209</v>
       </c>
@@ -2082,7 +2071,7 @@
         <v>48081</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>209</v>
       </c>
@@ -2093,7 +2082,7 @@
         <v>43251</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>209</v>
       </c>
@@ -2104,7 +2093,7 @@
         <v>24868</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>209</v>
       </c>
@@ -2115,7 +2104,7 @@
         <v>7662</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>209</v>
       </c>
@@ -2126,7 +2115,7 @@
         <v>4462</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>209</v>
       </c>
@@ -2137,7 +2126,7 @@
         <v>4062</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>209</v>
       </c>
@@ -2148,7 +2137,7 @@
         <v>6623</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>209</v>
       </c>
@@ -2159,7 +2148,7 @@
         <v>13208</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>209</v>
       </c>
@@ -2170,7 +2159,7 @@
         <v>2748</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>209</v>
       </c>
@@ -2181,7 +2170,7 @@
         <v>2769</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>220</v>
       </c>
@@ -2192,7 +2181,7 @@
         <v>9805</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>220</v>
       </c>
@@ -2203,7 +2192,7 @@
         <v>34046</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>220</v>
       </c>
@@ -2214,7 +2203,7 @@
         <v>124792</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>220</v>
       </c>
@@ -2225,7 +2214,7 @@
         <v>14611</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>220</v>
       </c>
@@ -2236,7 +2225,7 @@
         <v>54582</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>220</v>
       </c>
@@ -2247,7 +2236,7 @@
         <v>3386</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>220</v>
       </c>
@@ -2258,7 +2247,7 @@
         <v>15275</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>220</v>
       </c>
@@ -2269,942 +2258,942 @@
         <v>12706</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>220</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>228</v>
+        <v>315</v>
       </c>
       <c r="C80" s="6">
         <v>10655</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>220</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C81" s="7">
         <v>21577</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>220</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C82" s="6">
         <v>17244</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>220</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C83" s="7">
         <v>3307</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>220</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C84" s="6">
         <v>12909</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>220</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C85" s="7">
         <v>4673</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>220</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C86" s="3">
         <v>15877</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
         <v>220</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C87" s="5">
         <v>10129</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>220</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C88" s="3">
         <v>6171</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="B89" s="4" t="s">
         <v>237</v>
-      </c>
-      <c r="B89" s="4" t="s">
-        <v>238</v>
       </c>
       <c r="C89" s="7">
         <v>4385</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C90" s="6">
         <v>5820</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C91" s="7">
         <v>5763</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C92" s="6">
         <v>10966</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C93" s="7">
         <v>46289</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C94" s="6">
         <v>13639</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C95" s="7">
         <v>3820</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C96" s="6">
         <v>2136</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C97" s="7">
         <v>4982</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C98" s="6">
         <v>5557</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C99" s="7">
         <v>8812</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C100" s="3">
         <v>10017</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C101" s="5">
         <v>4649</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C102" s="3">
         <v>6565</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="B103" s="4" t="s">
         <v>251</v>
-      </c>
-      <c r="B103" s="4" t="s">
-        <v>252</v>
       </c>
       <c r="C103" s="7">
         <v>36002</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C104" s="6">
         <v>2212</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C105" s="7">
         <v>4035</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C106" s="6">
         <v>5767</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C107" s="7">
         <v>56844</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C108" s="6">
         <v>18915</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C109" s="7">
         <v>23828</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C110" s="6">
         <v>60893</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C111" s="7">
         <v>4316</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C112" s="6">
         <v>37572</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C113" s="7">
         <v>50179</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C114" s="3">
         <v>9320</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C115" s="5">
         <v>30659</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C116" s="3">
         <v>21319</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C117" s="5">
         <v>3844</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C118" s="3">
         <v>16881</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="B119" s="4" t="s">
         <v>283</v>
-      </c>
-      <c r="B119" s="4" t="s">
-        <v>284</v>
       </c>
       <c r="C119" s="7">
         <v>5687</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C120" s="6">
         <v>6372</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C121" s="7">
         <v>7070</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C122" s="6">
         <v>5192</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C123" s="7">
         <v>4215</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C124" s="6">
         <v>11967</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C125" s="7">
         <v>36860</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C126" s="6">
         <v>2948</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C127" s="7">
         <v>4986</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C128" s="6">
         <v>8547</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C129" s="5">
         <v>11788</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C130" s="3">
         <v>20558</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C131" s="5">
         <v>8505</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C132" s="3">
         <v>6736</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="B133" s="4" t="s">
         <v>297</v>
-      </c>
-      <c r="B133" s="4" t="s">
-        <v>298</v>
       </c>
       <c r="C133" s="7">
         <v>48808</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C134" s="6">
         <v>5741</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C135" s="7">
         <v>10997</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C136" s="6">
         <v>13912</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C137" s="7">
         <v>11464</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C138" s="6">
         <v>45184</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C139" s="7">
         <v>2466</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C140" s="6">
         <v>5061</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C141" s="7">
         <v>113366</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C142" s="6">
         <v>34220</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C143" s="7">
         <v>14101</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C144" s="6">
         <v>10714</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B145" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C145" s="7">
         <v>3009</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C146" s="6">
         <v>24268</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C147" s="7">
         <v>48313</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C148" s="6">
         <v>20560</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="B149" s="4" t="s">
         <v>267</v>
-      </c>
-      <c r="B149" s="4" t="s">
-        <v>268</v>
       </c>
       <c r="C149" s="7">
         <v>37091</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C150" s="6">
         <v>142381</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B151" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C151" s="7">
         <v>11861</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C152" s="6">
         <v>17691</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B153" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C153" s="7">
         <v>12273</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C154" s="6">
         <v>177628</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B155" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C155" s="7">
         <v>465439</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C156" s="6">
         <v>168472</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B157" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C157" s="7">
         <v>23746</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C158" s="6">
         <v>69811</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B159" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C159" s="7">
         <v>125826</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C160" s="6">
         <v>145353</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B161" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C161" s="5">
         <v>323643</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C162" s="3">
         <v>8891</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B163" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C163" s="5">
         <v>70586</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C164" s="3">
         <v>114480</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="4" t="s">
         <v>72</v>
       </c>
@@ -3215,7 +3204,7 @@
         <v>2662</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>72</v>
       </c>
@@ -3226,7 +3215,7 @@
         <v>2486</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="4" t="s">
         <v>72</v>
       </c>
@@ -3237,7 +3226,7 @@
         <v>3334</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>72</v>
       </c>
@@ -3248,7 +3237,7 @@
         <v>6945</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="4" t="s">
         <v>72</v>
       </c>
@@ -3259,7 +3248,7 @@
         <v>2640</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>72</v>
       </c>
@@ -3270,7 +3259,7 @@
         <v>2913</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="4" t="s">
         <v>72</v>
       </c>
@@ -3281,7 +3270,7 @@
         <v>18476</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
         <v>72</v>
       </c>
@@ -3292,7 +3281,7 @@
         <v>2634</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="4" t="s">
         <v>72</v>
       </c>
@@ -3303,7 +3292,7 @@
         <v>3136</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
         <v>72</v>
       </c>
@@ -3314,7 +3303,7 @@
         <v>2534</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="4" t="s">
         <v>72</v>
       </c>
@@ -3325,7 +3314,7 @@
         <v>2562</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
         <v>72</v>
       </c>
@@ -3336,7 +3325,7 @@
         <v>5563</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="4" t="s">
         <v>72</v>
       </c>
@@ -3347,7 +3336,7 @@
         <v>13657</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>72</v>
       </c>
@@ -3358,7 +3347,7 @@
         <v>19707</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="4" t="s">
         <v>72</v>
       </c>
@@ -3369,7 +3358,7 @@
         <v>3857</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>87</v>
       </c>
@@ -3380,7 +3369,7 @@
         <v>49980</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="4" t="s">
         <v>87</v>
       </c>
@@ -3391,7 +3380,7 @@
         <v>16295</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>87</v>
       </c>
@@ -3402,7 +3391,7 @@
         <v>51707</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" s="4" t="s">
         <v>87</v>
       </c>
@@ -3413,7 +3402,7 @@
         <v>145883</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>87</v>
       </c>
@@ -3424,7 +3413,7 @@
         <v>42119</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" s="4" t="s">
         <v>87</v>
       </c>
@@ -3435,7 +3424,7 @@
         <v>117071</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>87</v>
       </c>
@@ -3446,7 +3435,7 @@
         <v>45450</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" s="4" t="s">
         <v>87</v>
       </c>
@@ -3457,7 +3446,7 @@
         <v>150490</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
         <v>87</v>
       </c>
@@ -3468,7 +3457,7 @@
         <v>49291</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" s="4" t="s">
         <v>87</v>
       </c>
@@ -3479,7 +3468,7 @@
         <v>75337</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
         <v>87</v>
       </c>
@@ -3490,7 +3479,7 @@
         <v>62239</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" s="4" t="s">
         <v>87</v>
       </c>
@@ -3501,7 +3490,7 @@
         <v>204547</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
         <v>87</v>
       </c>
@@ -3512,7 +3501,7 @@
         <v>60733</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="4" t="s">
         <v>87</v>
       </c>
@@ -3523,7 +3512,7 @@
         <v>62012</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
         <v>87</v>
       </c>
@@ -3534,7 +3523,7 @@
         <v>33990</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="4" t="s">
         <v>87</v>
       </c>
@@ -3545,7 +3534,7 @@
         <v>84679</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
         <v>87</v>
       </c>
@@ -3556,7 +3545,7 @@
         <v>72197</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" s="4" t="s">
         <v>87</v>
       </c>
@@ -3567,7 +3556,7 @@
         <v>267659</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
         <v>14</v>
       </c>
@@ -3578,7 +3567,7 @@
         <v>33446</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" s="4" t="s">
         <v>14</v>
       </c>
@@ -3589,7 +3578,7 @@
         <v>3723</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
         <v>14</v>
       </c>
@@ -3600,7 +3589,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" s="4" t="s">
         <v>14</v>
       </c>
@@ -3611,7 +3600,7 @@
         <v>13011</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
         <v>14</v>
       </c>
@@ -3622,7 +3611,7 @@
         <v>12998</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" s="4" t="s">
         <v>14</v>
       </c>
@@ -3633,7 +3622,7 @@
         <v>1245</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
         <v>14</v>
       </c>
@@ -3644,7 +3633,7 @@
         <v>4483</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" s="4" t="s">
         <v>14</v>
       </c>
@@ -3655,7 +3644,7 @@
         <v>6032</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
         <v>14</v>
       </c>
@@ -3666,7 +3655,7 @@
         <v>4811</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" s="4" t="s">
         <v>14</v>
       </c>
@@ -3677,7 +3666,7 @@
         <v>65382</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
         <v>14</v>
       </c>
@@ -3688,7 +3677,7 @@
         <v>6274</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" s="4" t="s">
         <v>14</v>
       </c>
@@ -3699,7 +3688,7 @@
         <v>19657</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
         <v>14</v>
       </c>
@@ -3710,7 +3699,7 @@
         <v>28931</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" s="4" t="s">
         <v>14</v>
       </c>
@@ -3721,7 +3710,7 @@
         <v>3870</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
         <v>14</v>
       </c>
@@ -3732,7 +3721,7 @@
         <v>1837</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" s="4" t="s">
         <v>14</v>
       </c>
@@ -3743,7 +3732,7 @@
         <v>3301</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
         <v>14</v>
       </c>
@@ -3754,7 +3743,7 @@
         <v>4992</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" s="4" t="s">
         <v>14</v>
       </c>
@@ -3765,7 +3754,7 @@
         <v>5203</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
         <v>14</v>
       </c>
@@ -3776,7 +3765,7 @@
         <v>10531</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" s="4" t="s">
         <v>2</v>
       </c>
@@ -3787,7 +3776,7 @@
         <v>12309</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
         <v>2</v>
       </c>
@@ -3798,7 +3787,7 @@
         <v>32574</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" s="4" t="s">
         <v>2</v>
       </c>
@@ -3809,7 +3798,7 @@
         <v>104930</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
         <v>2</v>
       </c>
@@ -3820,7 +3809,7 @@
         <v>19809</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" s="4" t="s">
         <v>2</v>
       </c>
@@ -3831,7 +3820,7 @@
         <v>9801</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
         <v>2</v>
       </c>
@@ -3842,7 +3831,7 @@
         <v>3013</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" s="4" t="s">
         <v>2</v>
       </c>
@@ -3853,7 +3842,7 @@
         <v>5421</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
         <v>2</v>
       </c>
@@ -3864,7 +3853,7 @@
         <v>14033</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" s="4" t="s">
         <v>2</v>
       </c>
@@ -3875,7 +3864,7 @@
         <v>39899</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
         <v>2</v>
       </c>
@@ -3886,7 +3875,7 @@
         <v>6886</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" s="4" t="s">
         <v>2</v>
       </c>
@@ -3897,7 +3886,7 @@
         <v>5827</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
         <v>105</v>
       </c>
@@ -3908,7 +3897,7 @@
         <v>31047</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" s="4" t="s">
         <v>105</v>
       </c>
@@ -3919,7 +3908,7 @@
         <v>11456</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
         <v>105</v>
       </c>
@@ -3930,7 +3919,7 @@
         <v>19658</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" s="4" t="s">
         <v>105</v>
       </c>
@@ -3941,7 +3930,7 @@
         <v>6290</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
         <v>105</v>
       </c>
@@ -3952,7 +3941,7 @@
         <v>24872</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" s="4" t="s">
         <v>105</v>
       </c>
@@ -3963,7 +3952,7 @@
         <v>20746</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
         <v>105</v>
       </c>
@@ -3974,7 +3963,7 @@
         <v>7557</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" s="4" t="s">
         <v>105</v>
       </c>
@@ -3985,7 +3974,7 @@
         <v>3361</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" s="2" t="s">
         <v>105</v>
       </c>
@@ -3996,7 +3985,7 @@
         <v>15631</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" s="4" t="s">
         <v>105</v>
       </c>
@@ -4007,7 +3996,7 @@
         <v>16829</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" s="2" t="s">
         <v>105</v>
       </c>
@@ -4018,7 +4007,7 @@
         <v>6846</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" s="4" t="s">
         <v>105</v>
       </c>
@@ -4029,7 +4018,7 @@
         <v>4750</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" s="2" t="s">
         <v>105</v>
       </c>
@@ -4040,7 +4029,7 @@
         <v>5696</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" s="4" t="s">
         <v>105</v>
       </c>
@@ -4051,7 +4040,7 @@
         <v>40464</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242" s="2" t="s">
         <v>105</v>
       </c>
@@ -4062,7 +4051,7 @@
         <v>17807</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243" s="4" t="s">
         <v>105</v>
       </c>
@@ -4073,7 +4062,7 @@
         <v>19595</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
         <v>105</v>
       </c>
@@ -4084,7 +4073,7 @@
         <v>51027</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245" s="4" t="s">
         <v>105</v>
       </c>
@@ -4095,7 +4084,7 @@
         <v>3155</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
         <v>105</v>
       </c>
@@ -4106,7 +4095,7 @@
         <v>33346</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" s="4" t="s">
         <v>105</v>
       </c>
@@ -4117,7 +4106,7 @@
         <v>30718</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
         <v>105</v>
       </c>
@@ -4128,7 +4117,7 @@
         <v>6410</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" s="4" t="s">
         <v>126</v>
       </c>
@@ -4139,7 +4128,7 @@
         <v>9880</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250" s="2" t="s">
         <v>126</v>
       </c>
@@ -4150,7 +4139,7 @@
         <v>15513</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251" s="4" t="s">
         <v>126</v>
       </c>
@@ -4161,7 +4150,7 @@
         <v>150993</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252" s="2" t="s">
         <v>126</v>
       </c>
@@ -4172,7 +4161,7 @@
         <v>68061</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253" s="4" t="s">
         <v>126</v>
       </c>
@@ -4183,7 +4172,7 @@
         <v>11761</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
         <v>126</v>
       </c>
@@ -4194,7 +4183,7 @@
         <v>58807</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" s="4" t="s">
         <v>126</v>
       </c>
@@ -4205,7 +4194,7 @@
         <v>44389</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
         <v>126</v>
       </c>
@@ -4216,7 +4205,7 @@
         <v>58420</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257" s="4" t="s">
         <v>126</v>
       </c>
@@ -4227,7 +4216,7 @@
         <v>23982</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
         <v>126</v>
       </c>
@@ -4238,7 +4227,7 @@
         <v>145155</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A259" s="4" t="s">
         <v>126</v>
       </c>
@@ -4249,7 +4238,7 @@
         <v>46141</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
         <v>126</v>
       </c>
@@ -4260,7 +4249,7 @@
         <v>106140</v>
       </c>
     </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261" s="4" t="s">
         <v>126</v>
       </c>
@@ -4271,7 +4260,7 @@
         <v>12050</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262" s="2" t="s">
         <v>139</v>
       </c>
@@ -4282,7 +4271,7 @@
         <v>24312</v>
       </c>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A263" s="4" t="s">
         <v>139</v>
       </c>
@@ -4293,7 +4282,7 @@
         <v>15930</v>
       </c>
     </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
         <v>139</v>
       </c>
@@ -4304,7 +4293,7 @@
         <v>9643</v>
       </c>
     </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A265" s="4" t="s">
         <v>139</v>
       </c>
@@ -4315,7 +4304,7 @@
         <v>18837</v>
       </c>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266" s="2" t="s">
         <v>139</v>
       </c>
@@ -4326,7 +4315,7 @@
         <v>8503</v>
       </c>
     </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A267" s="4" t="s">
         <v>139</v>
       </c>
@@ -4337,7 +4326,7 @@
         <v>12888</v>
       </c>
     </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
         <v>139</v>
       </c>
@@ -4348,7 +4337,7 @@
         <v>40424</v>
       </c>
     </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A269" s="4" t="s">
         <v>139</v>
       </c>
@@ -4359,7 +4348,7 @@
         <v>12744</v>
       </c>
     </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A270" s="2" t="s">
         <v>139</v>
       </c>
@@ -4370,7 +4359,7 @@
         <v>81831</v>
       </c>
     </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A271" s="4" t="s">
         <v>139</v>
       </c>
@@ -4381,7 +4370,7 @@
         <v>8379</v>
       </c>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A272" s="2" t="s">
         <v>34</v>
       </c>
@@ -4392,7 +4381,7 @@
         <v>11027</v>
       </c>
     </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A273" s="4" t="s">
         <v>34</v>
       </c>
@@ -4403,7 +4392,7 @@
         <v>7551</v>
       </c>
     </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A274" s="2" t="s">
         <v>34</v>
       </c>
@@ -4414,7 +4403,7 @@
         <v>42481</v>
       </c>
     </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A275" s="4" t="s">
         <v>34</v>
       </c>
@@ -4425,7 +4414,7 @@
         <v>3424</v>
       </c>
     </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A276" s="2" t="s">
         <v>34</v>
       </c>
@@ -4436,7 +4425,7 @@
         <v>7515</v>
       </c>
     </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A277" s="4" t="s">
         <v>34</v>
       </c>
@@ -4447,7 +4436,7 @@
         <v>13099</v>
       </c>
     </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A278" s="2" t="s">
         <v>34</v>
       </c>
@@ -4458,7 +4447,7 @@
         <v>6123</v>
       </c>
     </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A279" s="4" t="s">
         <v>34</v>
       </c>
@@ -4469,7 +4458,7 @@
         <v>14861</v>
       </c>
     </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A280" s="2" t="s">
         <v>34</v>
       </c>
@@ -4480,7 +4469,7 @@
         <v>8135</v>
       </c>
     </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A281" s="4" t="s">
         <v>34</v>
       </c>
@@ -4491,7 +4480,7 @@
         <v>6108</v>
       </c>
     </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A282" s="2" t="s">
         <v>34</v>
       </c>
@@ -4502,7 +4491,7 @@
         <v>6976</v>
       </c>
     </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A283" s="4" t="s">
         <v>34</v>
       </c>
@@ -4513,7 +4502,7 @@
         <v>18338</v>
       </c>
     </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A284" s="2" t="s">
         <v>34</v>
       </c>
@@ -4524,7 +4513,7 @@
         <v>13705</v>
       </c>
     </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A285" s="4" t="s">
         <v>34</v>
       </c>
@@ -4535,7 +4524,7 @@
         <v>49324</v>
       </c>
     </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A286" s="2" t="s">
         <v>48</v>
       </c>
@@ -4546,7 +4535,7 @@
         <v>5640</v>
       </c>
     </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A287" s="4" t="s">
         <v>48</v>
       </c>
@@ -4557,7 +4546,7 @@
         <v>8912</v>
       </c>
     </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A288" s="2" t="s">
         <v>48</v>
       </c>
@@ -4568,7 +4557,7 @@
         <v>13670</v>
       </c>
     </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A289" s="4" t="s">
         <v>48</v>
       </c>
@@ -4579,7 +4568,7 @@
         <v>15993</v>
       </c>
     </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A290" s="2" t="s">
         <v>48</v>
       </c>
@@ -4590,7 +4579,7 @@
         <v>23156</v>
       </c>
     </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A291" s="4" t="s">
         <v>48</v>
       </c>
@@ -4601,7 +4590,7 @@
         <v>17775</v>
       </c>
     </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A292" s="2" t="s">
         <v>48</v>
       </c>
@@ -4612,7 +4601,7 @@
         <v>9945</v>
       </c>
     </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A293" s="4" t="s">
         <v>48</v>
       </c>
@@ -4623,7 +4612,7 @@
         <v>8250</v>
       </c>
     </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A294" s="2" t="s">
         <v>48</v>
       </c>
@@ -4634,7 +4623,7 @@
         <v>12336</v>
       </c>
     </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A295" s="4" t="s">
         <v>48</v>
       </c>
@@ -4645,7 +4634,7 @@
         <v>8620</v>
       </c>
     </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A296" s="2" t="s">
         <v>48</v>
       </c>
@@ -4656,7 +4645,7 @@
         <v>7247</v>
       </c>
     </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A297" s="4" t="s">
         <v>48</v>
       </c>
@@ -4667,7 +4656,7 @@
         <v>2798</v>
       </c>
     </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A298" s="2" t="s">
         <v>48</v>
       </c>
@@ -4678,7 +4667,7 @@
         <v>9722</v>
       </c>
     </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A299" s="4" t="s">
         <v>48</v>
       </c>
@@ -4689,7 +4678,7 @@
         <v>10153</v>
       </c>
     </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A300" s="2" t="s">
         <v>48</v>
       </c>
@@ -4700,7 +4689,7 @@
         <v>6480</v>
       </c>
     </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A301" s="4" t="s">
         <v>48</v>
       </c>
@@ -4711,7 +4700,7 @@
         <v>14623</v>
       </c>
     </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A302" s="2" t="s">
         <v>48</v>
       </c>
@@ -4722,7 +4711,7 @@
         <v>12201</v>
       </c>
     </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A303" s="4" t="s">
         <v>48</v>
       </c>
@@ -4733,7 +4722,7 @@
         <v>5044</v>
       </c>
     </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A304" s="2" t="s">
         <v>48</v>
       </c>
@@ -4744,7 +4733,7 @@
         <v>4633</v>
       </c>
     </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A305" s="4" t="s">
         <v>48</v>
       </c>
@@ -4755,7 +4744,7 @@
         <v>7161</v>
       </c>
     </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A306" s="2" t="s">
         <v>48</v>
       </c>
@@ -4766,7 +4755,7 @@
         <v>24357</v>
       </c>
     </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A307" s="4" t="s">
         <v>48</v>
       </c>
@@ -4777,7 +4766,7 @@
         <v>5735</v>
       </c>
     </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A308" s="2" t="s">
         <v>48</v>
       </c>
@@ -4788,7 +4777,7 @@
         <v>92381</v>
       </c>
     </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A309" s="4" t="s">
         <v>48</v>
       </c>
@@ -4799,29 +4788,29 @@
         <v>8827</v>
       </c>
     </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A310" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B310" s="4" t="s">
         <v>313</v>
-      </c>
-      <c r="B310" s="4" t="s">
-        <v>314</v>
       </c>
       <c r="C310" s="4">
         <v>937311</v>
       </c>
     </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A311" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B311" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C311" s="4">
         <v>609436</v>
       </c>
     </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A312" s="8"/>
     </row>
   </sheetData>

</xml_diff>